<commit_message>
Check metadata using validation and evaluation via metapype
</commit_message>
<xml_diff>
--- a/webapp/static/evaluate.xlsx
+++ b/webapp/static/evaluate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jide/git/metadata-eml/webapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jide/git/metadata-eml/webapp/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DC23AA-9D23-D740-A85B-F6FE2275D6C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EC78AB-EB14-B74D-BC48-ECEF00FE1047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="-20040" windowWidth="36120" windowHeight="19100" xr2:uid="{006A8ECD-8FE2-ED42-8DC4-FA0074059980}"/>
+    <workbookView xWindow="1780" yWindow="-27920" windowWidth="36120" windowHeight="25260" xr2:uid="{006A8ECD-8FE2-ED42-8DC4-FA0074059980}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -128,9 +128,6 @@
     <t>abstract_02</t>
   </si>
   <si>
-    <t>Consider increasing the length of the dataset's &lt;b&gt;Abstract&lt;/b&gt;.</t>
-  </si>
-  <si>
     <t>Currently, shown if number of words &lt; 20.</t>
   </si>
   <si>
@@ -300,6 +297,147 @@
   </si>
   <si>
     <t>For Categorical attributes</t>
+  </si>
+  <si>
+    <t>responsible_party_04</t>
+  </si>
+  <si>
+    <t>Applies if first or middle name is provided, but no last name.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Last Name&lt;/b&gt; is required if First Name or Middle Name/Initial  is given.</t>
+  </si>
+  <si>
+    <t>geographic_coverage_03</t>
+  </si>
+  <si>
+    <t>West Bounding Coordinate</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;West Bounding Coordinate&lt;/b&gt; must be a decimal value between -180.0 and +180.0.</t>
+  </si>
+  <si>
+    <t>geographic_coverage_04</t>
+  </si>
+  <si>
+    <t>East Bounding Coordinate</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;East Bounding Coordinate&lt;/b&gt; must be a decimal value between -180.0 and +180.0.</t>
+  </si>
+  <si>
+    <t>geographic_coverage_05</t>
+  </si>
+  <si>
+    <t>North Bounding Coordinate</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;North Bounding Coordinate&lt;/b&gt; must be a decimal value between -90.0 and +90.0.</t>
+  </si>
+  <si>
+    <t>geographic_coverage_06</t>
+  </si>
+  <si>
+    <t>South Bounding Coordinate</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;South Bounding Coordinate&lt;/b&gt; must be a decimal value between -90.0 and +90.0.</t>
+  </si>
+  <si>
+    <t>methods_01</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>Method Steps</t>
+  </si>
+  <si>
+    <t>A dataset should define at least one &lt;b&gt;Method Step&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>project_01</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Project Title</t>
+  </si>
+  <si>
+    <t>The &lt;b&gt;Project Title&lt;/b&gt; is required.</t>
+  </si>
+  <si>
+    <t>project_02</t>
+  </si>
+  <si>
+    <t>Project Personnel</t>
+  </si>
+  <si>
+    <t>At least one &lt;b&gt;Project Personnel&lt;/b&gt; is required.</t>
+  </si>
+  <si>
+    <t>project_03</t>
+  </si>
+  <si>
+    <t>A dataset should define a &lt;b&gt;Project&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>other_entity_01</t>
+  </si>
+  <si>
+    <t>Other Entities</t>
+  </si>
+  <si>
+    <t>other_entity_02</t>
+  </si>
+  <si>
+    <t>Entity Type</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Entity Type&lt;/b&gt; is required.</t>
+  </si>
+  <si>
+    <t>Entity &lt;b&gt;Name&lt;/b&gt; is required.</t>
+  </si>
+  <si>
+    <t>other_entity_03</t>
+  </si>
+  <si>
+    <t>Entity Description</t>
+  </si>
+  <si>
+    <t>Entity &lt;b&gt;Description&lt;/b&gt; is highly recommended.</t>
+  </si>
+  <si>
+    <t>project_04</t>
+  </si>
+  <si>
+    <t>Funder Name</t>
+  </si>
+  <si>
+    <t>project_05</t>
+  </si>
+  <si>
+    <t>Award Title</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Funder Name&lt;/b&gt; is required.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Award Title&lt;/b&gt; is required.</t>
+  </si>
+  <si>
+    <t>contacts_01</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>At least one &lt;b&gt;Contact&lt;/b&gt; is required.</t>
+  </si>
+  <si>
+    <t>Consider increasing the length of the dataset's &lt;b&gt;Abstract&lt;/b&gt;. 20 or more words is a recommended length.</t>
   </si>
 </sst>
 </file>
@@ -663,17 +801,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F00D08-7E49-E44C-88BD-C093B08B860E}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="61.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="5" width="20.83203125" customWidth="1"/>
+    <col min="6" max="6" width="81.5" customWidth="1"/>
     <col min="7" max="7" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -828,30 +968,32 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>28</v>
@@ -866,21 +1008,19 @@
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
@@ -889,19 +1029,21 @@
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="2"/>
+        <v>134</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
@@ -910,19 +1052,19 @@
         <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>9</v>
@@ -931,19 +1073,19 @@
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>9</v>
@@ -952,107 +1094,107 @@
         <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
@@ -1061,19 +1203,19 @@
         <v>13</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
@@ -1082,41 +1224,41 @@
         <v>13</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1124,44 +1266,40 @@
         <v>13</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>77</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>12</v>
@@ -1170,21 +1308,19 @@
         <v>13</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>12</v>
@@ -1193,176 +1329,426 @@
         <v>13</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>88</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>88</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="D31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>